<commit_message>
final commit (I hope)
</commit_message>
<xml_diff>
--- a/files/employees.xlsx
+++ b/files/employees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -50,7 +50,22 @@
     <t>1</t>
   </si>
   <si>
+    <t>fired</t>
+  </si>
+  <si>
+    <t>Papov</t>
+  </si>
+  <si>
+    <t>Adel</t>
+  </si>
+  <si>
     <t>L1</t>
+  </si>
+  <si>
+    <t>сотрудник</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -102,7 +117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -186,6 +201,75 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="n">
+        <v>27489.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="n">
+        <v>31977.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="n">
+        <v>31977.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>